<commit_message>
updated benchmark test & benchmark results
</commit_message>
<xml_diff>
--- a/benchmark.xlsx
+++ b/benchmark.xlsx
@@ -141,12 +141,42 @@
         </r>
       </text>
     </comment>
+    <comment ref="H42" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="238"/>
+          </rPr>
+          <t>memory_get_peak_usage(FALSE)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I42" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="238"/>
+          </rPr>
+          <t>memory_get_usage(FALSE)</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="23">
   <si>
     <t>TEST 1</t>
   </si>
@@ -212,6 +242,9 @@
   </si>
   <si>
     <t>AR#3</t>
+  </si>
+  <si>
+    <t>AR#4</t>
   </si>
 </sst>
 </file>
@@ -566,10 +599,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J38"/>
+  <dimension ref="A1:J48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1344,9 +1377,20 @@
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
     </row>
+    <row r="30" spans="1:10">
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+      <c r="J30" s="1"/>
+    </row>
     <row r="31" spans="1:10">
       <c r="A31" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>13</v>
@@ -1398,33 +1442,33 @@
         <v>0</v>
       </c>
       <c r="B33" s="3">
-        <v>3.3</v>
+        <v>10.1</v>
       </c>
       <c r="C33" s="3">
-        <v>4.3</v>
+        <v>10.1</v>
       </c>
       <c r="D33" s="3">
-        <v>2.8</v>
+        <v>10.1</v>
       </c>
       <c r="E33" s="3">
-        <v>2.9</v>
+        <v>10.8</v>
       </c>
       <c r="F33" s="3">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="G33" s="3">
-        <f>AVERAGE(B33,C33,D33,E33,F33)</f>
-        <v>3.2599999999999993</v>
+        <f>AVERAGE(B33:F33)</f>
+        <v>10.219999999999999</v>
       </c>
       <c r="H33" s="3">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="I33" s="3">
-        <v>1.2</v>
+        <v>1.9</v>
       </c>
       <c r="J33" s="3">
         <f>MAX(H33:I33)</f>
-        <v>1.2</v>
+        <v>1.9</v>
       </c>
     </row>
     <row r="34" spans="1:10">
@@ -1432,33 +1476,33 @@
         <v>1</v>
       </c>
       <c r="B34" s="3">
-        <v>5.6</v>
+        <v>42.2</v>
       </c>
       <c r="C34" s="3">
-        <v>5.7</v>
+        <v>42.5</v>
       </c>
       <c r="D34" s="3">
-        <v>6.3</v>
+        <v>42.6</v>
       </c>
       <c r="E34" s="3">
-        <v>7.2</v>
+        <v>44.5</v>
       </c>
       <c r="F34" s="3">
-        <v>5.6</v>
+        <v>45.8</v>
       </c>
       <c r="G34" s="3">
-        <f>AVERAGE(B34,C34,D34,E34,F34)</f>
-        <v>6.08</v>
+        <f t="shared" ref="G34:G37" si="4">AVERAGE(B34:F34)</f>
+        <v>43.52</v>
       </c>
       <c r="H34" s="3">
-        <v>5.2</v>
+        <v>13.9</v>
       </c>
       <c r="I34" s="3">
-        <v>12.2</v>
+        <v>22.4</v>
       </c>
       <c r="J34" s="3">
-        <f t="shared" ref="J34:J37" si="4">MAX(H34:I34)</f>
-        <v>12.2</v>
+        <f t="shared" ref="J34:J37" si="5">MAX(H34:I34)</f>
+        <v>22.4</v>
       </c>
     </row>
     <row r="35" spans="1:10">
@@ -1466,33 +1510,33 @@
         <v>2</v>
       </c>
       <c r="B35" s="3">
-        <v>32.799999999999997</v>
+        <v>370.2</v>
       </c>
       <c r="C35" s="3">
-        <v>34.1</v>
+        <v>374.2</v>
       </c>
       <c r="D35" s="3">
-        <v>32.200000000000003</v>
+        <v>369</v>
       </c>
       <c r="E35" s="3">
-        <v>31.1</v>
+        <v>370.7</v>
       </c>
       <c r="F35" s="3">
-        <v>31.5</v>
+        <v>370.7</v>
       </c>
       <c r="G35" s="3">
-        <f>AVERAGE(B35,C35,D35,E35,F35)</f>
-        <v>32.340000000000003</v>
+        <f t="shared" si="4"/>
+        <v>370.96000000000004</v>
       </c>
       <c r="H35" s="3">
-        <v>87.9</v>
+        <v>176.6</v>
       </c>
       <c r="I35" s="3">
-        <v>108.8</v>
+        <v>164.3</v>
       </c>
       <c r="J35" s="3">
-        <f t="shared" si="4"/>
-        <v>108.8</v>
+        <f t="shared" si="5"/>
+        <v>176.6</v>
       </c>
     </row>
     <row r="36" spans="1:10">
@@ -1500,67 +1544,63 @@
         <v>3</v>
       </c>
       <c r="B36" s="3">
-        <v>294</v>
+        <v>3773.7</v>
       </c>
       <c r="C36" s="3">
-        <v>293.39999999999998</v>
+        <v>3794.9</v>
       </c>
       <c r="D36" s="3">
-        <v>288.8</v>
+        <v>3770.9</v>
       </c>
       <c r="E36" s="3">
-        <v>317.5</v>
+        <v>3811</v>
       </c>
       <c r="F36" s="3">
-        <v>285.8</v>
+        <v>3791.7</v>
       </c>
       <c r="G36" s="3">
-        <f>AVERAGE(B36,C36,D36,E36,F36)</f>
-        <v>295.89999999999998</v>
+        <f t="shared" si="4"/>
+        <v>3788.44</v>
       </c>
       <c r="H36" s="3">
-        <v>1229.7</v>
+        <v>1814.5</v>
       </c>
       <c r="I36" s="3">
-        <v>1117.2</v>
+        <v>1692.1</v>
       </c>
       <c r="J36" s="3">
-        <f t="shared" si="4"/>
-        <v>1229.7</v>
+        <f t="shared" si="5"/>
+        <v>1814.5</v>
       </c>
     </row>
     <row r="37" spans="1:10">
       <c r="A37" t="s">
         <v>4</v>
       </c>
-      <c r="B37" s="3">
-        <v>15322.7</v>
-      </c>
-      <c r="C37" s="3">
-        <v>15581.2</v>
-      </c>
+      <c r="B37" s="3"/>
+      <c r="C37" s="3"/>
       <c r="D37" s="3">
-        <v>15538.9</v>
+        <v>204081.7</v>
       </c>
       <c r="E37" s="3">
-        <v>15792</v>
+        <v>233939.1</v>
       </c>
       <c r="F37" s="3">
-        <v>15052.9</v>
+        <v>209042.2</v>
       </c>
       <c r="G37" s="3">
-        <f>AVERAGE(B37,C37,D37,E37,F37)</f>
-        <v>15457.539999999999</v>
+        <f t="shared" si="4"/>
+        <v>215687.66666666666</v>
       </c>
       <c r="H37" s="3">
-        <v>63807.7</v>
+        <v>99880.7</v>
       </c>
       <c r="I37" s="3">
-        <v>61226.6</v>
+        <v>94709.5</v>
       </c>
       <c r="J37" s="3">
-        <f t="shared" si="4"/>
-        <v>63807.7</v>
+        <f t="shared" si="5"/>
+        <v>99880.7</v>
       </c>
     </row>
     <row r="38" spans="1:10">
@@ -1583,17 +1623,336 @@
         <v>8</v>
       </c>
       <c r="H38" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J38" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10">
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
+      <c r="H39" s="1"/>
+      <c r="I39" s="1"/>
+      <c r="J39" s="1"/>
+    </row>
+    <row r="41" spans="1:10">
+      <c r="A41" t="s">
+        <v>7</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10">
+      <c r="B42" t="s">
+        <v>5</v>
+      </c>
+      <c r="C42" t="s">
+        <v>5</v>
+      </c>
+      <c r="D42" t="s">
+        <v>5</v>
+      </c>
+      <c r="E42" t="s">
+        <v>5</v>
+      </c>
+      <c r="F42" t="s">
+        <v>5</v>
+      </c>
+      <c r="G42" t="s">
+        <v>6</v>
+      </c>
+      <c r="H42" t="s">
+        <v>9</v>
+      </c>
+      <c r="I42" t="s">
+        <v>10</v>
+      </c>
+      <c r="J42" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10">
+      <c r="A43" t="s">
+        <v>0</v>
+      </c>
+      <c r="B43" s="3">
+        <v>3.3</v>
+      </c>
+      <c r="C43" s="3">
+        <v>4.3</v>
+      </c>
+      <c r="D43" s="3">
+        <v>2.8</v>
+      </c>
+      <c r="E43" s="3">
+        <v>3.9</v>
+      </c>
+      <c r="F43" s="3">
+        <v>3</v>
+      </c>
+      <c r="G43" s="3">
+        <f>AVERAGE(B43,C43,D43,E43,F43)</f>
+        <v>3.4599999999999995</v>
+      </c>
+      <c r="H43" s="3">
+        <v>0</v>
+      </c>
+      <c r="I43" s="3">
+        <v>1.2</v>
+      </c>
+      <c r="J43" s="3">
+        <f>MAX(H43:I43)</f>
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10">
+      <c r="A44" t="s">
+        <v>1</v>
+      </c>
+      <c r="B44" s="3">
+        <v>5.6</v>
+      </c>
+      <c r="C44" s="3">
+        <v>5.7</v>
+      </c>
+      <c r="D44" s="3">
+        <v>6.3</v>
+      </c>
+      <c r="E44" s="3">
+        <v>6.4</v>
+      </c>
+      <c r="F44" s="3">
+        <v>5.6</v>
+      </c>
+      <c r="G44" s="3">
+        <f>AVERAGE(B44,C44,D44,E44,F44)</f>
+        <v>5.92</v>
+      </c>
+      <c r="H44" s="3">
+        <v>5.2</v>
+      </c>
+      <c r="I44" s="3">
+        <v>12.2</v>
+      </c>
+      <c r="J44" s="3">
+        <f t="shared" ref="J44:J47" si="6">MAX(H44:I44)</f>
+        <v>12.2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10">
+      <c r="A45" t="s">
+        <v>2</v>
+      </c>
+      <c r="B45" s="3">
+        <v>32.799999999999997</v>
+      </c>
+      <c r="C45" s="3">
+        <v>34.1</v>
+      </c>
+      <c r="D45" s="3">
+        <v>32.200000000000003</v>
+      </c>
+      <c r="E45" s="3">
+        <v>37.200000000000003</v>
+      </c>
+      <c r="F45" s="3">
+        <v>31.5</v>
+      </c>
+      <c r="G45" s="3">
+        <f>AVERAGE(B45,C45,D45,E45,F45)</f>
+        <v>33.56</v>
+      </c>
+      <c r="H45" s="3">
+        <v>87.9</v>
+      </c>
+      <c r="I45" s="3">
+        <v>108.8</v>
+      </c>
+      <c r="J45" s="3">
+        <f t="shared" si="6"/>
+        <v>108.8</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10">
+      <c r="A46" t="s">
+        <v>3</v>
+      </c>
+      <c r="B46" s="3">
+        <v>294</v>
+      </c>
+      <c r="C46" s="3">
+        <v>293.39999999999998</v>
+      </c>
+      <c r="D46" s="3">
+        <v>288.8</v>
+      </c>
+      <c r="E46" s="3">
+        <v>330.8</v>
+      </c>
+      <c r="F46" s="3">
+        <v>285.8</v>
+      </c>
+      <c r="G46" s="3">
+        <f>AVERAGE(B46,C46,D46,E46,F46)</f>
+        <v>298.56</v>
+      </c>
+      <c r="H46" s="3">
+        <v>1229.7</v>
+      </c>
+      <c r="I46" s="3">
+        <v>1085.8</v>
+      </c>
+      <c r="J46" s="3">
+        <f t="shared" si="6"/>
+        <v>1229.7</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10">
+      <c r="A47" t="s">
+        <v>4</v>
+      </c>
+      <c r="B47" s="3">
+        <v>15322.7</v>
+      </c>
+      <c r="C47" s="3">
+        <v>15581.2</v>
+      </c>
+      <c r="D47" s="3">
+        <v>15538.9</v>
+      </c>
+      <c r="E47" s="3">
+        <v>15792</v>
+      </c>
+      <c r="F47" s="3">
+        <v>15052.9</v>
+      </c>
+      <c r="G47" s="3">
+        <f>AVERAGE(B47,C47,D47,E47,F47)</f>
+        <v>15457.539999999999</v>
+      </c>
+      <c r="H47" s="3">
+        <v>63807.7</v>
+      </c>
+      <c r="I47" s="3">
+        <v>61226.6</v>
+      </c>
+      <c r="J47" s="3">
+        <f t="shared" si="6"/>
+        <v>63807.7</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10">
+      <c r="B48" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H48" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I38" s="1" t="s">
+      <c r="I48" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J38" s="1" t="s">
+      <c r="J48" s="1" t="s">
         <v>19</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B3:F3">
+    <cfRule type="colorScale" priority="71">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B4:F4">
+    <cfRule type="colorScale" priority="70">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B5:F5">
+    <cfRule type="colorScale" priority="69">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B6:F6">
+    <cfRule type="colorScale" priority="68">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B7:F7">
+    <cfRule type="colorScale" priority="67">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B13:F13">
     <cfRule type="colorScale" priority="61">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -1605,19 +1964,19 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B4:F4">
+  <conditionalFormatting sqref="B14:F14">
     <cfRule type="colorScale" priority="60">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
         <cfvo type="max" val="0"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B5:F5">
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B15:F15">
     <cfRule type="colorScale" priority="59">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -1629,7 +1988,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B6:F6">
+  <conditionalFormatting sqref="B16:F16">
     <cfRule type="colorScale" priority="58">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -1641,7 +2000,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B7:F7">
+  <conditionalFormatting sqref="B17:F17">
     <cfRule type="colorScale" priority="57">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -1653,7 +2012,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B13:F13">
+  <conditionalFormatting sqref="B43:F43">
     <cfRule type="colorScale" priority="51">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -1665,7 +2024,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B14:F14">
+  <conditionalFormatting sqref="B44:F44">
     <cfRule type="colorScale" priority="50">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -1677,7 +2036,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B15:F15">
+  <conditionalFormatting sqref="B45:F45">
     <cfRule type="colorScale" priority="49">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -1689,7 +2048,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B16:F16">
+  <conditionalFormatting sqref="B46:F46">
     <cfRule type="colorScale" priority="48">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -1701,7 +2060,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B17:F17">
+  <conditionalFormatting sqref="B47:F47">
     <cfRule type="colorScale" priority="47">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -1713,8 +2072,308 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="H3:I3">
+    <cfRule type="colorScale" priority="35">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H4:I4">
+    <cfRule type="colorScale" priority="34">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H5:I5">
+    <cfRule type="colorScale" priority="33">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H6:I6">
+    <cfRule type="colorScale" priority="32">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H7:I7">
+    <cfRule type="colorScale" priority="31">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H47:I47">
+    <cfRule type="colorScale" priority="30">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H46:I46">
+    <cfRule type="colorScale" priority="29">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H45:I45">
+    <cfRule type="colorScale" priority="28">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H44:I44">
+    <cfRule type="colorScale" priority="27">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H43:I43">
+    <cfRule type="colorScale" priority="26">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H13:I13">
+    <cfRule type="colorScale" priority="25">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H14:I14">
+    <cfRule type="colorScale" priority="24">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H15:I15">
+    <cfRule type="colorScale" priority="23">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H16:I16">
+    <cfRule type="colorScale" priority="22">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H17:I17">
+    <cfRule type="colorScale" priority="21">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B23:F23">
+    <cfRule type="colorScale" priority="20">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B24:F24">
+    <cfRule type="colorScale" priority="19">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B25:F25">
+    <cfRule type="colorScale" priority="18">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B26:F26">
+    <cfRule type="colorScale" priority="17">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B27:F27">
+    <cfRule type="colorScale" priority="16">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H23:I23">
+    <cfRule type="colorScale" priority="15">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H24:I24">
+    <cfRule type="colorScale" priority="14">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H25:I25">
+    <cfRule type="colorScale" priority="13">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H26:I26">
+    <cfRule type="colorScale" priority="12">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H27:I27">
+    <cfRule type="colorScale" priority="11">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="B33:F33">
-    <cfRule type="colorScale" priority="41">
+    <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -1726,7 +2385,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B34:F34">
-    <cfRule type="colorScale" priority="40">
+    <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -1738,7 +2397,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B35:F35">
-    <cfRule type="colorScale" priority="39">
+    <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -1750,7 +2409,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B36:F36">
-    <cfRule type="colorScale" priority="38">
+    <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -1762,67 +2421,55 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B37:F37">
-    <cfRule type="colorScale" priority="37">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H3:I3">
-    <cfRule type="colorScale" priority="25">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H4:I4">
-    <cfRule type="colorScale" priority="24">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H5:I5">
-    <cfRule type="colorScale" priority="23">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H6:I6">
-    <cfRule type="colorScale" priority="22">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H7:I7">
-    <cfRule type="colorScale" priority="21">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H33:I33">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H34:I34">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H35:I35">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H36:I36">
+    <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -1834,234 +2481,6 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H37:I37">
-    <cfRule type="colorScale" priority="20">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H36:I36">
-    <cfRule type="colorScale" priority="19">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H35:I35">
-    <cfRule type="colorScale" priority="18">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H34:I34">
-    <cfRule type="colorScale" priority="17">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H33:I33">
-    <cfRule type="colorScale" priority="16">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H13:I13">
-    <cfRule type="colorScale" priority="15">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H14:I14">
-    <cfRule type="colorScale" priority="14">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H15:I15">
-    <cfRule type="colorScale" priority="13">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H16:I16">
-    <cfRule type="colorScale" priority="12">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H17:I17">
-    <cfRule type="colorScale" priority="11">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B23:F23">
-    <cfRule type="colorScale" priority="10">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B24:F24">
-    <cfRule type="colorScale" priority="9">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B25:F25">
-    <cfRule type="colorScale" priority="8">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B26:F26">
-    <cfRule type="colorScale" priority="7">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B27:F27">
-    <cfRule type="colorScale" priority="6">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H23:I23">
-    <cfRule type="colorScale" priority="5">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H24:I24">
-    <cfRule type="colorScale" priority="4">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H25:I25">
-    <cfRule type="colorScale" priority="3">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H26:I26">
-    <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H27:I27">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min" val="0"/>

</xml_diff>

<commit_message>
updated benchmark test (result: ActiveRecord takes less memory, but more time)
</commit_message>
<xml_diff>
--- a/benchmark.xlsx
+++ b/benchmark.xlsx
@@ -171,12 +171,42 @@
         </r>
       </text>
     </comment>
+    <comment ref="H52" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="238"/>
+          </rPr>
+          <t>memory_get_peak_usage(FALSE)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I52" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="238"/>
+          </rPr>
+          <t>memory_get_usage(FALSE)</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="24">
   <si>
     <t>TEST 1</t>
   </si>
@@ -245,6 +275,9 @@
   </si>
   <si>
     <t>AR#4</t>
+  </si>
+  <si>
+    <t>AR#5</t>
   </si>
 </sst>
 </file>
@@ -599,10 +632,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J48"/>
+  <dimension ref="A1:J58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="O45" sqref="O45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1643,9 +1676,20 @@
       <c r="I39" s="1"/>
       <c r="J39" s="1"/>
     </row>
+    <row r="40" spans="1:10">
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
+      <c r="G40" s="1"/>
+      <c r="H40" s="1"/>
+      <c r="I40" s="1"/>
+      <c r="J40" s="1"/>
+    </row>
     <row r="41" spans="1:10">
       <c r="A41" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>13</v>
@@ -1697,33 +1741,29 @@
         <v>0</v>
       </c>
       <c r="B43" s="3">
-        <v>3.3</v>
+        <v>11.8</v>
       </c>
       <c r="C43" s="3">
-        <v>4.3</v>
+        <v>13.5</v>
       </c>
       <c r="D43" s="3">
-        <v>2.8</v>
-      </c>
-      <c r="E43" s="3">
-        <v>3.9</v>
-      </c>
-      <c r="F43" s="3">
-        <v>3</v>
-      </c>
+        <v>13.1</v>
+      </c>
+      <c r="E43" s="3"/>
+      <c r="F43" s="3"/>
       <c r="G43" s="3">
-        <f>AVERAGE(B43,C43,D43,E43,F43)</f>
-        <v>3.4599999999999995</v>
+        <f>AVERAGE(B43:F43)</f>
+        <v>12.799999999999999</v>
       </c>
       <c r="H43" s="3">
-        <v>0</v>
+        <v>1.2</v>
       </c>
       <c r="I43" s="3">
-        <v>1.2</v>
+        <v>2.4</v>
       </c>
       <c r="J43" s="3">
         <f>MAX(H43:I43)</f>
-        <v>1.2</v>
+        <v>2.4</v>
       </c>
     </row>
     <row r="44" spans="1:10">
@@ -1731,33 +1771,29 @@
         <v>1</v>
       </c>
       <c r="B44" s="3">
-        <v>5.6</v>
+        <v>45.5</v>
       </c>
       <c r="C44" s="3">
-        <v>5.7</v>
+        <v>53</v>
       </c>
       <c r="D44" s="3">
-        <v>6.3</v>
-      </c>
-      <c r="E44" s="3">
-        <v>6.4</v>
-      </c>
-      <c r="F44" s="3">
-        <v>5.6</v>
-      </c>
+        <v>52.1</v>
+      </c>
+      <c r="E44" s="3"/>
+      <c r="F44" s="3"/>
       <c r="G44" s="3">
-        <f>AVERAGE(B44,C44,D44,E44,F44)</f>
-        <v>5.92</v>
+        <f t="shared" ref="G44:G47" si="6">AVERAGE(B44:F44)</f>
+        <v>50.199999999999996</v>
       </c>
       <c r="H44" s="3">
-        <v>5.2</v>
+        <v>14.3</v>
       </c>
       <c r="I44" s="3">
-        <v>12.2</v>
+        <v>30.2</v>
       </c>
       <c r="J44" s="3">
-        <f t="shared" ref="J44:J47" si="6">MAX(H44:I44)</f>
-        <v>12.2</v>
+        <f t="shared" ref="J44:J47" si="7">MAX(H44:I44)</f>
+        <v>30.2</v>
       </c>
     </row>
     <row r="45" spans="1:10">
@@ -1765,33 +1801,29 @@
         <v>2</v>
       </c>
       <c r="B45" s="3">
-        <v>32.799999999999997</v>
+        <v>428.2</v>
       </c>
       <c r="C45" s="3">
-        <v>34.1</v>
+        <v>459.1</v>
       </c>
       <c r="D45" s="3">
-        <v>32.200000000000003</v>
-      </c>
-      <c r="E45" s="3">
-        <v>37.200000000000003</v>
-      </c>
-      <c r="F45" s="3">
-        <v>31.5</v>
-      </c>
+        <v>454.2</v>
+      </c>
+      <c r="E45" s="3"/>
+      <c r="F45" s="3"/>
       <c r="G45" s="3">
-        <f>AVERAGE(B45,C45,D45,E45,F45)</f>
-        <v>33.56</v>
+        <f t="shared" si="6"/>
+        <v>447.16666666666669</v>
       </c>
       <c r="H45" s="3">
-        <v>87.9</v>
+        <v>166.8</v>
       </c>
       <c r="I45" s="3">
-        <v>108.8</v>
+        <v>149.4</v>
       </c>
       <c r="J45" s="3">
-        <f t="shared" si="6"/>
-        <v>108.8</v>
+        <f t="shared" si="7"/>
+        <v>166.8</v>
       </c>
     </row>
     <row r="46" spans="1:10">
@@ -1799,33 +1831,29 @@
         <v>3</v>
       </c>
       <c r="B46" s="3">
-        <v>294</v>
+        <v>4420</v>
       </c>
       <c r="C46" s="3">
-        <v>293.39999999999998</v>
+        <v>4675.8999999999996</v>
       </c>
       <c r="D46" s="3">
-        <v>288.8</v>
-      </c>
-      <c r="E46" s="3">
-        <v>330.8</v>
-      </c>
-      <c r="F46" s="3">
-        <v>285.8</v>
-      </c>
+        <v>4712.8999999999996</v>
+      </c>
+      <c r="E46" s="3"/>
+      <c r="F46" s="3"/>
       <c r="G46" s="3">
-        <f>AVERAGE(B46,C46,D46,E46,F46)</f>
-        <v>298.56</v>
+        <f t="shared" si="6"/>
+        <v>4602.9333333333334</v>
       </c>
       <c r="H46" s="3">
-        <v>1229.7</v>
+        <v>1748.2</v>
       </c>
       <c r="I46" s="3">
-        <v>1085.8</v>
+        <v>1601</v>
       </c>
       <c r="J46" s="3">
-        <f t="shared" si="6"/>
-        <v>1229.7</v>
+        <f t="shared" si="7"/>
+        <v>1748.2</v>
       </c>
     </row>
     <row r="47" spans="1:10">
@@ -1833,33 +1861,29 @@
         <v>4</v>
       </c>
       <c r="B47" s="3">
-        <v>15322.7</v>
+        <v>222051.1</v>
       </c>
       <c r="C47" s="3">
-        <v>15581.2</v>
+        <v>240430.2</v>
       </c>
       <c r="D47" s="3">
-        <v>15538.9</v>
-      </c>
-      <c r="E47" s="3">
-        <v>15792</v>
-      </c>
-      <c r="F47" s="3">
-        <v>15052.9</v>
-      </c>
+        <v>239697.1</v>
+      </c>
+      <c r="E47" s="3"/>
+      <c r="F47" s="3"/>
       <c r="G47" s="3">
-        <f>AVERAGE(B47,C47,D47,E47,F47)</f>
-        <v>15457.539999999999</v>
+        <f t="shared" si="6"/>
+        <v>234059.46666666667</v>
       </c>
       <c r="H47" s="3">
-        <v>63807.7</v>
+        <v>91885.2</v>
       </c>
       <c r="I47" s="3">
-        <v>61226.6</v>
+        <v>86717.8</v>
       </c>
       <c r="J47" s="3">
-        <f t="shared" si="6"/>
-        <v>63807.7</v>
+        <f t="shared" si="7"/>
+        <v>91885.2</v>
       </c>
     </row>
     <row r="48" spans="1:10">
@@ -1882,17 +1906,336 @@
         <v>8</v>
       </c>
       <c r="H48" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I48" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J48" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10">
+      <c r="B49" s="1"/>
+      <c r="C49" s="1"/>
+      <c r="D49" s="1"/>
+      <c r="E49" s="1"/>
+      <c r="F49" s="1"/>
+      <c r="G49" s="1"/>
+      <c r="H49" s="1"/>
+      <c r="I49" s="1"/>
+      <c r="J49" s="1"/>
+    </row>
+    <row r="51" spans="1:10">
+      <c r="A51" t="s">
+        <v>7</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F51" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10">
+      <c r="B52" t="s">
+        <v>5</v>
+      </c>
+      <c r="C52" t="s">
+        <v>5</v>
+      </c>
+      <c r="D52" t="s">
+        <v>5</v>
+      </c>
+      <c r="E52" t="s">
+        <v>5</v>
+      </c>
+      <c r="F52" t="s">
+        <v>5</v>
+      </c>
+      <c r="G52" t="s">
+        <v>6</v>
+      </c>
+      <c r="H52" t="s">
+        <v>9</v>
+      </c>
+      <c r="I52" t="s">
+        <v>10</v>
+      </c>
+      <c r="J52" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10">
+      <c r="A53" t="s">
+        <v>0</v>
+      </c>
+      <c r="B53" s="3">
+        <v>3.3</v>
+      </c>
+      <c r="C53" s="3">
+        <v>4.3</v>
+      </c>
+      <c r="D53" s="3">
+        <v>2.8</v>
+      </c>
+      <c r="E53" s="3">
+        <v>3.9</v>
+      </c>
+      <c r="F53" s="3">
+        <v>3</v>
+      </c>
+      <c r="G53" s="3">
+        <f>AVERAGE(B53,C53,D53,E53,F53)</f>
+        <v>3.4599999999999995</v>
+      </c>
+      <c r="H53" s="3">
+        <v>0</v>
+      </c>
+      <c r="I53" s="3">
+        <v>1.2</v>
+      </c>
+      <c r="J53" s="3">
+        <f>MAX(H53:I53)</f>
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10">
+      <c r="A54" t="s">
+        <v>1</v>
+      </c>
+      <c r="B54" s="3">
+        <v>5.6</v>
+      </c>
+      <c r="C54" s="3">
+        <v>5.7</v>
+      </c>
+      <c r="D54" s="3">
+        <v>6.3</v>
+      </c>
+      <c r="E54" s="3">
+        <v>6.4</v>
+      </c>
+      <c r="F54" s="3">
+        <v>5.6</v>
+      </c>
+      <c r="G54" s="3">
+        <f>AVERAGE(B54,C54,D54,E54,F54)</f>
+        <v>5.92</v>
+      </c>
+      <c r="H54" s="3">
+        <v>5.2</v>
+      </c>
+      <c r="I54" s="3">
+        <v>12.2</v>
+      </c>
+      <c r="J54" s="3">
+        <f t="shared" ref="J54:J57" si="8">MAX(H54:I54)</f>
+        <v>12.2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10">
+      <c r="A55" t="s">
+        <v>2</v>
+      </c>
+      <c r="B55" s="3">
+        <v>32.799999999999997</v>
+      </c>
+      <c r="C55" s="3">
+        <v>34.1</v>
+      </c>
+      <c r="D55" s="3">
+        <v>32.200000000000003</v>
+      </c>
+      <c r="E55" s="3">
+        <v>37.200000000000003</v>
+      </c>
+      <c r="F55" s="3">
+        <v>31.5</v>
+      </c>
+      <c r="G55" s="3">
+        <f>AVERAGE(B55,C55,D55,E55,F55)</f>
+        <v>33.56</v>
+      </c>
+      <c r="H55" s="3">
+        <v>87.9</v>
+      </c>
+      <c r="I55" s="3">
+        <v>108.8</v>
+      </c>
+      <c r="J55" s="3">
+        <f t="shared" si="8"/>
+        <v>108.8</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10">
+      <c r="A56" t="s">
+        <v>3</v>
+      </c>
+      <c r="B56" s="3">
+        <v>294</v>
+      </c>
+      <c r="C56" s="3">
+        <v>293.39999999999998</v>
+      </c>
+      <c r="D56" s="3">
+        <v>288.8</v>
+      </c>
+      <c r="E56" s="3">
+        <v>330.8</v>
+      </c>
+      <c r="F56" s="3">
+        <v>285.8</v>
+      </c>
+      <c r="G56" s="3">
+        <f>AVERAGE(B56,C56,D56,E56,F56)</f>
+        <v>298.56</v>
+      </c>
+      <c r="H56" s="3">
+        <v>1229.7</v>
+      </c>
+      <c r="I56" s="3">
+        <v>1085.8</v>
+      </c>
+      <c r="J56" s="3">
+        <f t="shared" si="8"/>
+        <v>1229.7</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10">
+      <c r="A57" t="s">
+        <v>4</v>
+      </c>
+      <c r="B57" s="3">
+        <v>15322.7</v>
+      </c>
+      <c r="C57" s="3">
+        <v>15581.2</v>
+      </c>
+      <c r="D57" s="3">
+        <v>15538.9</v>
+      </c>
+      <c r="E57" s="3">
+        <v>15792</v>
+      </c>
+      <c r="F57" s="3">
+        <v>15052.9</v>
+      </c>
+      <c r="G57" s="3">
+        <f>AVERAGE(B57,C57,D57,E57,F57)</f>
+        <v>15457.539999999999</v>
+      </c>
+      <c r="H57" s="3">
+        <v>63807.7</v>
+      </c>
+      <c r="I57" s="3">
+        <v>61226.6</v>
+      </c>
+      <c r="J57" s="3">
+        <f t="shared" si="8"/>
+        <v>63807.7</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10">
+      <c r="B58" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G58" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H58" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I48" s="1" t="s">
+      <c r="I58" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J48" s="1" t="s">
+      <c r="J58" s="1" t="s">
         <v>19</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B3:F3">
+    <cfRule type="colorScale" priority="81">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B4:F4">
+    <cfRule type="colorScale" priority="80">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B5:F5">
+    <cfRule type="colorScale" priority="79">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B6:F6">
+    <cfRule type="colorScale" priority="78">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B7:F7">
+    <cfRule type="colorScale" priority="77">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B13:F13">
     <cfRule type="colorScale" priority="71">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -1904,19 +2247,19 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B4:F4">
+  <conditionalFormatting sqref="B14:F14">
     <cfRule type="colorScale" priority="70">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
         <cfvo type="max" val="0"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B5:F5">
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B15:F15">
     <cfRule type="colorScale" priority="69">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -1928,7 +2271,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B6:F6">
+  <conditionalFormatting sqref="B16:F16">
     <cfRule type="colorScale" priority="68">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -1940,7 +2283,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B7:F7">
+  <conditionalFormatting sqref="B17:F17">
     <cfRule type="colorScale" priority="67">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -1952,7 +2295,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B13:F13">
+  <conditionalFormatting sqref="B53:F53">
     <cfRule type="colorScale" priority="61">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -1964,7 +2307,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B14:F14">
+  <conditionalFormatting sqref="B54:F54">
     <cfRule type="colorScale" priority="60">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -1976,7 +2319,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B15:F15">
+  <conditionalFormatting sqref="B55:F55">
     <cfRule type="colorScale" priority="59">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -1988,7 +2331,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B16:F16">
+  <conditionalFormatting sqref="B56:F56">
     <cfRule type="colorScale" priority="58">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -2000,7 +2343,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B17:F17">
+  <conditionalFormatting sqref="B57:F57">
     <cfRule type="colorScale" priority="57">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -2012,8 +2355,428 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="H3:I3">
+    <cfRule type="colorScale" priority="45">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H4:I4">
+    <cfRule type="colorScale" priority="44">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H5:I5">
+    <cfRule type="colorScale" priority="43">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H6:I6">
+    <cfRule type="colorScale" priority="42">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H7:I7">
+    <cfRule type="colorScale" priority="41">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H57:I57">
+    <cfRule type="colorScale" priority="40">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H56:I56">
+    <cfRule type="colorScale" priority="39">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H55:I55">
+    <cfRule type="colorScale" priority="38">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H54:I54">
+    <cfRule type="colorScale" priority="37">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H53:I53">
+    <cfRule type="colorScale" priority="36">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H13:I13">
+    <cfRule type="colorScale" priority="35">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H14:I14">
+    <cfRule type="colorScale" priority="34">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H15:I15">
+    <cfRule type="colorScale" priority="33">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H16:I16">
+    <cfRule type="colorScale" priority="32">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H17:I17">
+    <cfRule type="colorScale" priority="31">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B23:F23">
+    <cfRule type="colorScale" priority="30">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B24:F24">
+    <cfRule type="colorScale" priority="29">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B25:F25">
+    <cfRule type="colorScale" priority="28">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B26:F26">
+    <cfRule type="colorScale" priority="27">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B27:F27">
+    <cfRule type="colorScale" priority="26">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H23:I23">
+    <cfRule type="colorScale" priority="25">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H24:I24">
+    <cfRule type="colorScale" priority="24">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H25:I25">
+    <cfRule type="colorScale" priority="23">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H26:I26">
+    <cfRule type="colorScale" priority="22">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H27:I27">
+    <cfRule type="colorScale" priority="21">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B33:F33">
+    <cfRule type="colorScale" priority="20">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B34:F34">
+    <cfRule type="colorScale" priority="19">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B35:F35">
+    <cfRule type="colorScale" priority="18">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B36:F36">
+    <cfRule type="colorScale" priority="17">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B37:F37">
+    <cfRule type="colorScale" priority="16">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H33:I33">
+    <cfRule type="colorScale" priority="15">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H34:I34">
+    <cfRule type="colorScale" priority="14">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H35:I35">
+    <cfRule type="colorScale" priority="13">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H36:I36">
+    <cfRule type="colorScale" priority="12">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H37:I37">
+    <cfRule type="colorScale" priority="11">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="B43:F43">
-    <cfRule type="colorScale" priority="51">
+    <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -2025,7 +2788,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B44:F44">
-    <cfRule type="colorScale" priority="50">
+    <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -2037,7 +2800,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B45:F45">
-    <cfRule type="colorScale" priority="49">
+    <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -2049,7 +2812,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B46:F46">
-    <cfRule type="colorScale" priority="48">
+    <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -2061,67 +2824,55 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B47:F47">
-    <cfRule type="colorScale" priority="47">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H3:I3">
-    <cfRule type="colorScale" priority="35">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H4:I4">
-    <cfRule type="colorScale" priority="34">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H5:I5">
-    <cfRule type="colorScale" priority="33">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H6:I6">
-    <cfRule type="colorScale" priority="32">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H7:I7">
-    <cfRule type="colorScale" priority="31">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H43:I43">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H44:I44">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H45:I45">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H46:I46">
+    <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -2133,354 +2884,6 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H47:I47">
-    <cfRule type="colorScale" priority="30">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H46:I46">
-    <cfRule type="colorScale" priority="29">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H45:I45">
-    <cfRule type="colorScale" priority="28">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H44:I44">
-    <cfRule type="colorScale" priority="27">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H43:I43">
-    <cfRule type="colorScale" priority="26">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H13:I13">
-    <cfRule type="colorScale" priority="25">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H14:I14">
-    <cfRule type="colorScale" priority="24">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H15:I15">
-    <cfRule type="colorScale" priority="23">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H16:I16">
-    <cfRule type="colorScale" priority="22">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H17:I17">
-    <cfRule type="colorScale" priority="21">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B23:F23">
-    <cfRule type="colorScale" priority="20">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B24:F24">
-    <cfRule type="colorScale" priority="19">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B25:F25">
-    <cfRule type="colorScale" priority="18">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B26:F26">
-    <cfRule type="colorScale" priority="17">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B27:F27">
-    <cfRule type="colorScale" priority="16">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H23:I23">
-    <cfRule type="colorScale" priority="15">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H24:I24">
-    <cfRule type="colorScale" priority="14">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H25:I25">
-    <cfRule type="colorScale" priority="13">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H26:I26">
-    <cfRule type="colorScale" priority="12">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H27:I27">
-    <cfRule type="colorScale" priority="11">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B33:F33">
-    <cfRule type="colorScale" priority="10">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B34:F34">
-    <cfRule type="colorScale" priority="9">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B35:F35">
-    <cfRule type="colorScale" priority="8">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B36:F36">
-    <cfRule type="colorScale" priority="7">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B37:F37">
-    <cfRule type="colorScale" priority="6">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H33:I33">
-    <cfRule type="colorScale" priority="5">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H34:I34">
-    <cfRule type="colorScale" priority="4">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H35:I35">
-    <cfRule type="colorScale" priority="3">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H36:I36">
-    <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H37:I37">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min" val="0"/>

</xml_diff>